<commit_message>
Updated isolation host data
</commit_message>
<xml_diff>
--- a/tabular/genus/erythro-refseqs-side-data.xlsx
+++ b/tabular/genus/erythro-refseqs-side-data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10215"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/comparative/DNAss/Parvoviridae-GLUE/tabular/genus/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/comparative/DNA/Parvovirus-GLUE/tabular/genus/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF0B8C34-AF35-904A-8970-6A5C85B913F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBE474F3-19AA-F548-BFBE-1649C5270FAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="18380" yWindow="2760" windowWidth="28800" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="51">
   <si>
     <t>virus_name</t>
   </si>
@@ -160,6 +160,24 @@
   </si>
   <si>
     <t>ErythroPV-Hyaena-1</t>
+  </si>
+  <si>
+    <t>Macaca mulatta</t>
+  </si>
+  <si>
+    <t>Macaca nemestrina</t>
+  </si>
+  <si>
+    <t>Tamias sibiricus</t>
+  </si>
+  <si>
+    <t>Bos taurus</t>
+  </si>
+  <si>
+    <t>Macaca fascicularis</t>
+  </si>
+  <si>
+    <t>Phoca vitulina</t>
   </si>
 </sst>
 </file>
@@ -2416,7 +2434,7 @@
   <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="A1:M10"/>
+      <selection activeCell="B6" sqref="A1:M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2484,7 +2502,7 @@
         <v>11</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>32</v>
@@ -2566,7 +2584,7 @@
         <v>17</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>32</v>
@@ -2607,7 +2625,7 @@
         <v>20</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>32</v>
@@ -2648,7 +2666,7 @@
         <v>23</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>32</v>
@@ -2689,7 +2707,7 @@
         <v>26</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>32</v>
+        <v>47</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>32</v>
@@ -2730,7 +2748,7 @@
         <v>29</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>32</v>

</xml_diff>

<commit_message>
Refactor - feature locations
</commit_message>
<xml_diff>
--- a/tabular/genus/erythro-refseqs-side-data.xlsx
+++ b/tabular/genus/erythro-refseqs-side-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/comparative/DNA/Parvovirus-GLUE/tabular/genus/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBE474F3-19AA-F548-BFBE-1649C5270FAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ABCC2C3-BC2F-154D-805F-CC8E4894F9A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="18380" yWindow="2760" windowWidth="28800" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2434,7 +2434,7 @@
   <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="A1:M10"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>